<commit_message>
chore(data): add 2025-2 data files ('25.07.20)
</commit_message>
<xml_diff>
--- a/data/2025년 2학기 정규 시간표.xlsx
+++ b/data/2025년 2학기 정규 시간표.xlsx
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1445"/>
+  <dimension ref="A1:N1446"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5094,8 +5094,16 @@
           <t>한숙정</t>
         </is>
       </c>
-      <c r="J78" t="inlineStr"/>
-      <c r="K78" t="inlineStr"/>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>화5~6,금5~6</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>다니엘관404호(大)강의실</t>
+        </is>
+      </c>
       <c r="L78" t="inlineStr">
         <is>
           <t>간호대학</t>
@@ -5150,8 +5158,16 @@
           <t>한숙정</t>
         </is>
       </c>
-      <c r="J79" t="inlineStr"/>
-      <c r="K79" t="inlineStr"/>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>화7~8,금7~8</t>
+        </is>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>다니엘관405호(大)강의실</t>
+        </is>
+      </c>
       <c r="L79" t="inlineStr">
         <is>
           <t>간호대학</t>
@@ -41936,12 +41952,12 @@
       </c>
       <c r="J693" t="inlineStr">
         <is>
-          <t>월6~7</t>
+          <t>월3</t>
         </is>
       </c>
       <c r="K693" t="inlineStr">
         <is>
-          <t>제3과학관209호(문제중심학습)</t>
+          <t>미지정</t>
         </is>
       </c>
       <c r="L693" t="inlineStr">
@@ -43146,8 +43162,16 @@
           <t>박일호</t>
         </is>
       </c>
-      <c r="J713" t="inlineStr"/>
-      <c r="K713" t="inlineStr"/>
+      <c r="J713" t="inlineStr">
+        <is>
+          <t>월6~7</t>
+        </is>
+      </c>
+      <c r="K713" t="inlineStr">
+        <is>
+          <t>다니엘관303호(中)강의실</t>
+        </is>
+      </c>
       <c r="L713" t="inlineStr">
         <is>
           <t>약학대학</t>
@@ -43198,16 +43222,8 @@
           <t>이바울</t>
         </is>
       </c>
-      <c r="J714" t="inlineStr">
-        <is>
-          <t>금2~3</t>
-        </is>
-      </c>
-      <c r="K714" t="inlineStr">
-        <is>
-          <t>제3과학관209호(문제중심학습)</t>
-        </is>
-      </c>
+      <c r="J714" t="inlineStr"/>
+      <c r="K714" t="inlineStr"/>
       <c r="L714" t="inlineStr">
         <is>
           <t>약학대학</t>
@@ -47000,12 +47016,12 @@
       </c>
       <c r="J778" t="inlineStr">
         <is>
-          <t>화4~5,수3</t>
+          <t>화1~3</t>
         </is>
       </c>
       <c r="K778" t="inlineStr">
         <is>
-          <t>바울관312호강의실</t>
+          <t>제3과학관418호(약학강의실)</t>
         </is>
       </c>
       <c r="L778" t="inlineStr">
@@ -47360,12 +47376,12 @@
       </c>
       <c r="J784" t="inlineStr">
         <is>
-          <t>수6~8</t>
+          <t>월6~8</t>
         </is>
       </c>
       <c r="K784" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>제3과학관418호(약학강의실)</t>
         </is>
       </c>
       <c r="L784" t="inlineStr">
@@ -49508,12 +49524,12 @@
       </c>
       <c r="J818" t="inlineStr">
         <is>
-          <t>수1~2</t>
+          <t>월5~7</t>
         </is>
       </c>
       <c r="K818" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>바울관312호강의실</t>
         </is>
       </c>
       <c r="L818" t="inlineStr">
@@ -49521,7 +49537,11 @@
           <t>창의융합대학</t>
         </is>
       </c>
-      <c r="M818" t="inlineStr"/>
+      <c r="M818" t="inlineStr">
+        <is>
+          <t>교직필수</t>
+        </is>
+      </c>
       <c r="N818" t="inlineStr"/>
     </row>
     <row r="819">
@@ -49566,22 +49586,18 @@
           <t>명지원</t>
         </is>
       </c>
-      <c r="J819" t="inlineStr">
-        <is>
-          <t>목8~9</t>
-        </is>
-      </c>
-      <c r="K819" t="inlineStr">
-        <is>
-          <t>미지정</t>
-        </is>
-      </c>
+      <c r="J819" t="inlineStr"/>
+      <c r="K819" t="inlineStr"/>
       <c r="L819" t="inlineStr">
         <is>
           <t>창의융합대학</t>
         </is>
       </c>
-      <c r="M819" t="inlineStr"/>
+      <c r="M819" t="inlineStr">
+        <is>
+          <t>교직필수</t>
+        </is>
+      </c>
       <c r="N819" t="inlineStr"/>
     </row>
     <row r="820">
@@ -49626,22 +49642,18 @@
           <t>박완성</t>
         </is>
       </c>
-      <c r="J820" t="inlineStr">
-        <is>
-          <t>월8~9</t>
-        </is>
-      </c>
-      <c r="K820" t="inlineStr">
-        <is>
-          <t>미지정</t>
-        </is>
-      </c>
+      <c r="J820" t="inlineStr"/>
+      <c r="K820" t="inlineStr"/>
       <c r="L820" t="inlineStr">
         <is>
           <t>창의융합대학</t>
         </is>
       </c>
-      <c r="M820" t="inlineStr"/>
+      <c r="M820" t="inlineStr">
+        <is>
+          <t>교직필수</t>
+        </is>
+      </c>
       <c r="N820" t="inlineStr"/>
     </row>
     <row r="821">
@@ -51049,11 +51061,7 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I842" t="inlineStr">
-        <is>
-          <t>미지정</t>
-        </is>
-      </c>
+      <c r="I842" t="inlineStr"/>
       <c r="J842" t="inlineStr"/>
       <c r="K842" t="inlineStr"/>
       <c r="L842" t="inlineStr">
@@ -51265,7 +51273,11 @@
           <t>창의융합대학</t>
         </is>
       </c>
-      <c r="M845" t="inlineStr"/>
+      <c r="M845" t="inlineStr">
+        <is>
+          <t>사회과학영역</t>
+        </is>
+      </c>
       <c r="N845" t="inlineStr"/>
     </row>
     <row r="846">
@@ -56105,7 +56117,11 @@
           <t>창의융합대학</t>
         </is>
       </c>
-      <c r="M917" t="inlineStr"/>
+      <c r="M917" t="inlineStr">
+        <is>
+          <t>사회과학영역</t>
+        </is>
+      </c>
       <c r="N917" t="inlineStr"/>
     </row>
     <row r="918">
@@ -56481,13 +56497,17 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I923" t="inlineStr">
-        <is>
-          <t>미지정</t>
-        </is>
-      </c>
-      <c r="J923" t="inlineStr"/>
-      <c r="K923" t="inlineStr"/>
+      <c r="I923" t="inlineStr"/>
+      <c r="J923" t="inlineStr">
+        <is>
+          <t>수2~4</t>
+        </is>
+      </c>
+      <c r="K923" t="inlineStr">
+        <is>
+          <t>바울관214호강의실</t>
+        </is>
+      </c>
       <c r="L923" t="inlineStr">
         <is>
           <t>창의융합대학</t>
@@ -56537,13 +56557,17 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I924" t="inlineStr">
+      <c r="I924" t="inlineStr"/>
+      <c r="J924" t="inlineStr">
+        <is>
+          <t>목6~9</t>
+        </is>
+      </c>
+      <c r="K924" t="inlineStr">
         <is>
           <t>미지정</t>
         </is>
       </c>
-      <c r="J924" t="inlineStr"/>
-      <c r="K924" t="inlineStr"/>
       <c r="L924" t="inlineStr">
         <is>
           <t>창의융합대학</t>
@@ -57196,12 +57220,12 @@
       </c>
       <c r="J934" t="inlineStr">
         <is>
-          <t>화7~9</t>
+          <t>월5~7</t>
         </is>
       </c>
       <c r="K934" t="inlineStr">
         <is>
-          <t>제3과학관418호(약학강의실)</t>
+          <t>미지정</t>
         </is>
       </c>
       <c r="L934" t="inlineStr">
@@ -57262,8 +57286,16 @@
           <t>백숭기</t>
         </is>
       </c>
-      <c r="J935" t="inlineStr"/>
-      <c r="K935" t="inlineStr"/>
+      <c r="J935" t="inlineStr">
+        <is>
+          <t>목5~7</t>
+        </is>
+      </c>
+      <c r="K935" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L935" t="inlineStr">
         <is>
           <t>창의융합대학</t>
@@ -60920,12 +60952,12 @@
       </c>
       <c r="J991" t="inlineStr">
         <is>
-          <t>화5~6</t>
+          <t>수5~7</t>
         </is>
       </c>
       <c r="K991" t="inlineStr">
         <is>
-          <t>제3과학관418호(약학강의실)</t>
+          <t>미지정</t>
         </is>
       </c>
       <c r="L991" t="inlineStr">
@@ -61260,12 +61292,12 @@
       </c>
       <c r="J996" t="inlineStr">
         <is>
-          <t>월6~8</t>
+          <t>수6~8</t>
         </is>
       </c>
       <c r="K996" t="inlineStr">
         <is>
-          <t>제3과학관418호(약학강의실)</t>
+          <t>미지정</t>
         </is>
       </c>
       <c r="L996" t="inlineStr">
@@ -61328,12 +61360,12 @@
       </c>
       <c r="J997" t="inlineStr">
         <is>
-          <t>수5~8</t>
+          <t>월2~4</t>
         </is>
       </c>
       <c r="K997" t="inlineStr">
         <is>
-          <t>제3과학관307호(약학과실험실2)</t>
+          <t>미지정</t>
         </is>
       </c>
       <c r="L997" t="inlineStr">
@@ -61613,7 +61645,11 @@
           <t>창의융합대학</t>
         </is>
       </c>
-      <c r="M1001" t="inlineStr"/>
+      <c r="M1001" t="inlineStr">
+        <is>
+          <t>자연과학영역</t>
+        </is>
+      </c>
       <c r="N1001" t="inlineStr"/>
     </row>
     <row r="1002">
@@ -62533,11 +62569,7 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I1015" t="inlineStr">
-        <is>
-          <t>미지정</t>
-        </is>
-      </c>
+      <c r="I1015" t="inlineStr"/>
       <c r="J1015" t="inlineStr">
         <is>
           <t>목7~9</t>
@@ -62553,7 +62585,11 @@
           <t>창의융합대학</t>
         </is>
       </c>
-      <c r="M1015" t="inlineStr"/>
+      <c r="M1015" t="inlineStr">
+        <is>
+          <t>인문예술영역</t>
+        </is>
+      </c>
       <c r="N1015" t="inlineStr"/>
     </row>
     <row r="1016">
@@ -62876,12 +62912,12 @@
       </c>
       <c r="J1020" t="inlineStr">
         <is>
-          <t>화1~3</t>
+          <t>화6~8</t>
         </is>
       </c>
       <c r="K1020" t="inlineStr">
         <is>
-          <t>제3과학관418호(약학강의실)</t>
+          <t>미지정</t>
         </is>
       </c>
       <c r="L1020" t="inlineStr">
@@ -86671,17 +86707,17 @@
     <row r="1414">
       <c r="A1414" t="inlineStr">
         <is>
-          <t>1649</t>
+          <t>1815</t>
         </is>
       </c>
       <c r="B1414" t="inlineStr">
         <is>
-          <t>1004656</t>
+          <t>1004176</t>
         </is>
       </c>
       <c r="C1414" t="inlineStr">
         <is>
-          <t>중국문화와 언어</t>
+          <t>일본문화와 언어</t>
         </is>
       </c>
       <c r="D1414" t="inlineStr">
@@ -86705,21 +86741,9 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I1414" t="inlineStr">
-        <is>
-          <t>박민수</t>
-        </is>
-      </c>
-      <c r="J1414" t="inlineStr">
-        <is>
-          <t>월6~8</t>
-        </is>
-      </c>
-      <c r="K1414" t="inlineStr">
-        <is>
-          <t>바울관413호식음료실습실</t>
-        </is>
-      </c>
+      <c r="I1414" t="inlineStr"/>
+      <c r="J1414" t="inlineStr"/>
+      <c r="K1414" t="inlineStr"/>
       <c r="L1414" t="inlineStr">
         <is>
           <t>창의융합대학</t>
@@ -86731,17 +86755,17 @@
     <row r="1415">
       <c r="A1415" t="inlineStr">
         <is>
-          <t>488</t>
+          <t>1649</t>
         </is>
       </c>
       <c r="B1415" t="inlineStr">
         <is>
-          <t>1006788</t>
+          <t>1004656</t>
         </is>
       </c>
       <c r="C1415" t="inlineStr">
         <is>
-          <t>항공서비스커뮤니케이션</t>
+          <t>중국문화와 언어</t>
         </is>
       </c>
       <c r="D1415" t="inlineStr">
@@ -86756,7 +86780,7 @@
       </c>
       <c r="F1415" t="inlineStr">
         <is>
-          <t>전공필수</t>
+          <t>전공선택</t>
         </is>
       </c>
       <c r="G1415" t="inlineStr"/>
@@ -86767,12 +86791,12 @@
       </c>
       <c r="I1415" t="inlineStr">
         <is>
-          <t>이현주</t>
+          <t>박민수</t>
         </is>
       </c>
       <c r="J1415" t="inlineStr">
         <is>
-          <t>수3~5</t>
+          <t>월6~8</t>
         </is>
       </c>
       <c r="K1415" t="inlineStr">
@@ -86791,17 +86815,17 @@
     <row r="1416">
       <c r="A1416" t="inlineStr">
         <is>
-          <t>494</t>
+          <t>488</t>
         </is>
       </c>
       <c r="B1416" t="inlineStr">
         <is>
-          <t>1006074</t>
+          <t>1006788</t>
         </is>
       </c>
       <c r="C1416" t="inlineStr">
         <is>
-          <t>인생설계와 진로 II</t>
+          <t>항공서비스커뮤니케이션</t>
         </is>
       </c>
       <c r="D1416" t="inlineStr">
@@ -86811,33 +86835,33 @@
       </c>
       <c r="E1416" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F1416" t="inlineStr">
         <is>
-          <t>교양필수</t>
+          <t>전공필수</t>
         </is>
       </c>
       <c r="G1416" t="inlineStr"/>
       <c r="H1416" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I1416" t="inlineStr">
         <is>
-          <t>김민주</t>
+          <t>이현주</t>
         </is>
       </c>
       <c r="J1416" t="inlineStr">
         <is>
-          <t>화9</t>
+          <t>수3~5</t>
         </is>
       </c>
       <c r="K1416" t="inlineStr">
         <is>
-          <t>바울관401호항공실습실</t>
+          <t>바울관413호식음료실습실</t>
         </is>
       </c>
       <c r="L1416" t="inlineStr">
@@ -86851,7 +86875,7 @@
     <row r="1417">
       <c r="A1417" t="inlineStr">
         <is>
-          <t>495</t>
+          <t>494</t>
         </is>
       </c>
       <c r="B1417" t="inlineStr">
@@ -86887,7 +86911,7 @@
       </c>
       <c r="I1417" t="inlineStr">
         <is>
-          <t>박민수</t>
+          <t>김민주</t>
         </is>
       </c>
       <c r="J1417" t="inlineStr">
@@ -86897,7 +86921,7 @@
       </c>
       <c r="K1417" t="inlineStr">
         <is>
-          <t>바울관402호강의실</t>
+          <t>바울관401호항공실습실</t>
         </is>
       </c>
       <c r="L1417" t="inlineStr">
@@ -86911,7 +86935,7 @@
     <row r="1418">
       <c r="A1418" t="inlineStr">
         <is>
-          <t>496</t>
+          <t>495</t>
         </is>
       </c>
       <c r="B1418" t="inlineStr">
@@ -86947,7 +86971,7 @@
       </c>
       <c r="I1418" t="inlineStr">
         <is>
-          <t>유예진</t>
+          <t>박민수</t>
         </is>
       </c>
       <c r="J1418" t="inlineStr">
@@ -86957,7 +86981,7 @@
       </c>
       <c r="K1418" t="inlineStr">
         <is>
-          <t>바울관413호식음료실습실</t>
+          <t>바울관402호강의실</t>
         </is>
       </c>
       <c r="L1418" t="inlineStr">
@@ -86971,7 +86995,7 @@
     <row r="1419">
       <c r="A1419" t="inlineStr">
         <is>
-          <t>505</t>
+          <t>496</t>
         </is>
       </c>
       <c r="B1419" t="inlineStr">
@@ -87007,7 +87031,7 @@
       </c>
       <c r="I1419" t="inlineStr">
         <is>
-          <t>이효성</t>
+          <t>유예진</t>
         </is>
       </c>
       <c r="J1419" t="inlineStr">
@@ -87017,7 +87041,7 @@
       </c>
       <c r="K1419" t="inlineStr">
         <is>
-          <t>바울관403호강의실</t>
+          <t>바울관413호식음료실습실</t>
         </is>
       </c>
       <c r="L1419" t="inlineStr">
@@ -87031,7 +87055,7 @@
     <row r="1420">
       <c r="A1420" t="inlineStr">
         <is>
-          <t>506</t>
+          <t>505</t>
         </is>
       </c>
       <c r="B1420" t="inlineStr">
@@ -87067,7 +87091,7 @@
       </c>
       <c r="I1420" t="inlineStr">
         <is>
-          <t>안병삼</t>
+          <t>이효성</t>
         </is>
       </c>
       <c r="J1420" t="inlineStr">
@@ -87077,7 +87101,7 @@
       </c>
       <c r="K1420" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>바울관403호강의실</t>
         </is>
       </c>
       <c r="L1420" t="inlineStr">
@@ -87091,17 +87115,17 @@
     <row r="1421">
       <c r="A1421" t="inlineStr">
         <is>
-          <t>511</t>
+          <t>506</t>
         </is>
       </c>
       <c r="B1421" t="inlineStr">
         <is>
-          <t>1001121</t>
+          <t>1006074</t>
         </is>
       </c>
       <c r="C1421" t="inlineStr">
         <is>
-          <t>역사와문화</t>
+          <t>인생설계와 진로 II</t>
         </is>
       </c>
       <c r="D1421" t="inlineStr">
@@ -87119,29 +87143,25 @@
           <t>교양필수</t>
         </is>
       </c>
-      <c r="G1421" t="inlineStr">
-        <is>
-          <t>핵심교양</t>
-        </is>
-      </c>
+      <c r="G1421" t="inlineStr"/>
       <c r="H1421" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I1421" t="inlineStr">
         <is>
-          <t>김영수</t>
+          <t>안병삼</t>
         </is>
       </c>
       <c r="J1421" t="inlineStr">
         <is>
-          <t>월1~2</t>
+          <t>화9</t>
         </is>
       </c>
       <c r="K1421" t="inlineStr">
         <is>
-          <t>신학관201호강의실</t>
+          <t>미지정</t>
         </is>
       </c>
       <c r="L1421" t="inlineStr">
@@ -87149,27 +87169,23 @@
           <t>창의융합대학</t>
         </is>
       </c>
-      <c r="M1421" t="inlineStr">
-        <is>
-          <t>핵심교양</t>
-        </is>
-      </c>
+      <c r="M1421" t="inlineStr"/>
       <c r="N1421" t="inlineStr"/>
     </row>
     <row r="1422">
       <c r="A1422" t="inlineStr">
         <is>
-          <t>517</t>
+          <t>511</t>
         </is>
       </c>
       <c r="B1422" t="inlineStr">
         <is>
-          <t>1002330</t>
+          <t>1001121</t>
         </is>
       </c>
       <c r="C1422" t="inlineStr">
         <is>
-          <t>서비스경영론</t>
+          <t>역사와문화</t>
         </is>
       </c>
       <c r="D1422" t="inlineStr">
@@ -87184,28 +87200,32 @@
       </c>
       <c r="F1422" t="inlineStr">
         <is>
-          <t>전공선택</t>
-        </is>
-      </c>
-      <c r="G1422" t="inlineStr"/>
+          <t>교양필수</t>
+        </is>
+      </c>
+      <c r="G1422" t="inlineStr">
+        <is>
+          <t>핵심교양</t>
+        </is>
+      </c>
       <c r="H1422" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I1422" t="inlineStr">
         <is>
-          <t>이효성</t>
+          <t>김영수</t>
         </is>
       </c>
       <c r="J1422" t="inlineStr">
         <is>
-          <t>수2~4</t>
+          <t>월1~2</t>
         </is>
       </c>
       <c r="K1422" t="inlineStr">
         <is>
-          <t>바울관403호강의실</t>
+          <t>신학관201호강의실</t>
         </is>
       </c>
       <c r="L1422" t="inlineStr">
@@ -87213,23 +87233,27 @@
           <t>창의융합대학</t>
         </is>
       </c>
-      <c r="M1422" t="inlineStr"/>
+      <c r="M1422" t="inlineStr">
+        <is>
+          <t>핵심교양</t>
+        </is>
+      </c>
       <c r="N1422" t="inlineStr"/>
     </row>
     <row r="1423">
       <c r="A1423" t="inlineStr">
         <is>
-          <t>518</t>
+          <t>517</t>
         </is>
       </c>
       <c r="B1423" t="inlineStr">
         <is>
-          <t>1006789</t>
+          <t>1002330</t>
         </is>
       </c>
       <c r="C1423" t="inlineStr">
         <is>
-          <t>중국어문법</t>
+          <t>서비스경영론</t>
         </is>
       </c>
       <c r="D1423" t="inlineStr">
@@ -87255,12 +87279,12 @@
       </c>
       <c r="I1423" t="inlineStr">
         <is>
-          <t>박민수</t>
+          <t>이효성</t>
         </is>
       </c>
       <c r="J1423" t="inlineStr">
         <is>
-          <t>목2~4</t>
+          <t>수2~4</t>
         </is>
       </c>
       <c r="K1423" t="inlineStr">
@@ -87279,17 +87303,17 @@
     <row r="1424">
       <c r="A1424" t="inlineStr">
         <is>
-          <t>523</t>
+          <t>518</t>
         </is>
       </c>
       <c r="B1424" t="inlineStr">
         <is>
-          <t>1007126</t>
+          <t>1006789</t>
         </is>
       </c>
       <c r="C1424" t="inlineStr">
         <is>
-          <t>초급 일본어 회화</t>
+          <t>중국어문법</t>
         </is>
       </c>
       <c r="D1424" t="inlineStr">
@@ -87313,15 +87337,19 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I1424" t="inlineStr"/>
+      <c r="I1424" t="inlineStr">
+        <is>
+          <t>박민수</t>
+        </is>
+      </c>
       <c r="J1424" t="inlineStr">
         <is>
-          <t>월4~6</t>
+          <t>목2~4</t>
         </is>
       </c>
       <c r="K1424" t="inlineStr">
         <is>
-          <t>바울관413호식음료실습실</t>
+          <t>바울관403호강의실</t>
         </is>
       </c>
       <c r="L1424" t="inlineStr">
@@ -87335,17 +87363,17 @@
     <row r="1425">
       <c r="A1425" t="inlineStr">
         <is>
-          <t>524</t>
+          <t>523</t>
         </is>
       </c>
       <c r="B1425" t="inlineStr">
         <is>
-          <t>1005044</t>
+          <t>1007126</t>
         </is>
       </c>
       <c r="C1425" t="inlineStr">
         <is>
-          <t>초급중국어회화</t>
+          <t>초급 일본어 회화</t>
         </is>
       </c>
       <c r="D1425" t="inlineStr">
@@ -87369,19 +87397,15 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I1425" t="inlineStr">
-        <is>
-          <t>안병삼</t>
-        </is>
-      </c>
+      <c r="I1425" t="inlineStr"/>
       <c r="J1425" t="inlineStr">
         <is>
-          <t>화2~4</t>
+          <t>월4~6</t>
         </is>
       </c>
       <c r="K1425" t="inlineStr">
         <is>
-          <t>에스라관313호강의실(보건관리과실습실)</t>
+          <t>바울관413호식음료실습실</t>
         </is>
       </c>
       <c r="L1425" t="inlineStr">
@@ -87390,26 +87414,22 @@
         </is>
       </c>
       <c r="M1425" t="inlineStr"/>
-      <c r="N1425" t="inlineStr">
-        <is>
-          <t>(팀티칭)</t>
-        </is>
-      </c>
+      <c r="N1425" t="inlineStr"/>
     </row>
     <row r="1426">
       <c r="A1426" t="inlineStr">
         <is>
-          <t>1651</t>
+          <t>524</t>
         </is>
       </c>
       <c r="B1426" t="inlineStr">
         <is>
-          <t>1006790</t>
+          <t>1005044</t>
         </is>
       </c>
       <c r="C1426" t="inlineStr">
         <is>
-          <t>필수일본어문법</t>
+          <t>초급중국어회화</t>
         </is>
       </c>
       <c r="D1426" t="inlineStr">
@@ -87435,17 +87455,17 @@
       </c>
       <c r="I1426" t="inlineStr">
         <is>
-          <t>유예진</t>
+          <t>안병삼</t>
         </is>
       </c>
       <c r="J1426" t="inlineStr">
         <is>
-          <t>화5~7</t>
+          <t>화2~4</t>
         </is>
       </c>
       <c r="K1426" t="inlineStr">
         <is>
-          <t>바울관403호강의실</t>
+          <t>에스라관313호강의실(보건관리과실습실)</t>
         </is>
       </c>
       <c r="L1426" t="inlineStr">
@@ -87454,22 +87474,26 @@
         </is>
       </c>
       <c r="M1426" t="inlineStr"/>
-      <c r="N1426" t="inlineStr"/>
+      <c r="N1426" t="inlineStr">
+        <is>
+          <t>(팀티칭)</t>
+        </is>
+      </c>
     </row>
     <row r="1427">
       <c r="A1427" t="inlineStr">
         <is>
-          <t>491</t>
+          <t>1651</t>
         </is>
       </c>
       <c r="B1427" t="inlineStr">
         <is>
-          <t>1006848</t>
+          <t>1006790</t>
         </is>
       </c>
       <c r="C1427" t="inlineStr">
         <is>
-          <t>항공식음료실습</t>
+          <t>필수일본어문법</t>
         </is>
       </c>
       <c r="D1427" t="inlineStr">
@@ -87495,17 +87519,17 @@
       </c>
       <c r="I1427" t="inlineStr">
         <is>
-          <t>이현주</t>
+          <t>유예진</t>
         </is>
       </c>
       <c r="J1427" t="inlineStr">
         <is>
-          <t>수6~8</t>
+          <t>화5~7</t>
         </is>
       </c>
       <c r="K1427" t="inlineStr">
         <is>
-          <t>바울관413호식음료실습실</t>
+          <t>바울관403호강의실</t>
         </is>
       </c>
       <c r="L1427" t="inlineStr">
@@ -87519,17 +87543,17 @@
     <row r="1428">
       <c r="A1428" t="inlineStr">
         <is>
-          <t>1652</t>
+          <t>491</t>
         </is>
       </c>
       <c r="B1428" t="inlineStr">
         <is>
-          <t>1006952</t>
+          <t>1006848</t>
         </is>
       </c>
       <c r="C1428" t="inlineStr">
         <is>
-          <t>기초 일본어 번역</t>
+          <t>항공식음료실습</t>
         </is>
       </c>
       <c r="D1428" t="inlineStr">
@@ -87539,7 +87563,7 @@
       </c>
       <c r="E1428" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F1428" t="inlineStr">
@@ -87555,17 +87579,17 @@
       </c>
       <c r="I1428" t="inlineStr">
         <is>
-          <t>정세진</t>
+          <t>이현주</t>
         </is>
       </c>
       <c r="J1428" t="inlineStr">
         <is>
-          <t>화2~4</t>
+          <t>수6~8</t>
         </is>
       </c>
       <c r="K1428" t="inlineStr">
         <is>
-          <t>바울관402호강의실</t>
+          <t>바울관413호식음료실습실</t>
         </is>
       </c>
       <c r="L1428" t="inlineStr">
@@ -87579,17 +87603,17 @@
     <row r="1429">
       <c r="A1429" t="inlineStr">
         <is>
-          <t>498</t>
+          <t>1652</t>
         </is>
       </c>
       <c r="B1429" t="inlineStr">
         <is>
-          <t>1001785</t>
+          <t>1006952</t>
         </is>
       </c>
       <c r="C1429" t="inlineStr">
         <is>
-          <t>미디어중국어</t>
+          <t>기초 일본어 번역</t>
         </is>
       </c>
       <c r="D1429" t="inlineStr">
@@ -87615,12 +87639,12 @@
       </c>
       <c r="I1429" t="inlineStr">
         <is>
-          <t>박민수</t>
+          <t>정세진</t>
         </is>
       </c>
       <c r="J1429" t="inlineStr">
         <is>
-          <t>목6~8</t>
+          <t>화2~4</t>
         </is>
       </c>
       <c r="K1429" t="inlineStr">
@@ -87639,17 +87663,17 @@
     <row r="1430">
       <c r="A1430" t="inlineStr">
         <is>
-          <t>512</t>
+          <t>498</t>
         </is>
       </c>
       <c r="B1430" t="inlineStr">
         <is>
-          <t>1002329</t>
+          <t>1001785</t>
         </is>
       </c>
       <c r="C1430" t="inlineStr">
         <is>
-          <t>서비스마케팅</t>
+          <t>미디어중국어</t>
         </is>
       </c>
       <c r="D1430" t="inlineStr">
@@ -87675,17 +87699,17 @@
       </c>
       <c r="I1430" t="inlineStr">
         <is>
-          <t>김민주</t>
+          <t>박민수</t>
         </is>
       </c>
       <c r="J1430" t="inlineStr">
         <is>
-          <t>화6~8</t>
+          <t>목6~8</t>
         </is>
       </c>
       <c r="K1430" t="inlineStr">
         <is>
-          <t>바울관413호식음료실습실</t>
+          <t>바울관402호강의실</t>
         </is>
       </c>
       <c r="L1430" t="inlineStr">
@@ -87699,17 +87723,17 @@
     <row r="1431">
       <c r="A1431" t="inlineStr">
         <is>
-          <t>521</t>
+          <t>512</t>
         </is>
       </c>
       <c r="B1431" t="inlineStr">
         <is>
-          <t>1007125</t>
+          <t>1002329</t>
         </is>
       </c>
       <c r="C1431" t="inlineStr">
         <is>
-          <t>실용 중국어 회화</t>
+          <t>서비스마케팅</t>
         </is>
       </c>
       <c r="D1431" t="inlineStr">
@@ -87735,17 +87759,17 @@
       </c>
       <c r="I1431" t="inlineStr">
         <is>
-          <t>안병삼</t>
+          <t>김민주</t>
         </is>
       </c>
       <c r="J1431" t="inlineStr">
         <is>
-          <t>목2~4</t>
+          <t>화6~8</t>
         </is>
       </c>
       <c r="K1431" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>바울관413호식음료실습실</t>
         </is>
       </c>
       <c r="L1431" t="inlineStr">
@@ -87759,17 +87783,17 @@
     <row r="1432">
       <c r="A1432" t="inlineStr">
         <is>
-          <t>499</t>
+          <t>521</t>
         </is>
       </c>
       <c r="B1432" t="inlineStr">
         <is>
-          <t>1002912</t>
+          <t>1007125</t>
         </is>
       </c>
       <c r="C1432" t="inlineStr">
         <is>
-          <t>실용일본어회화</t>
+          <t>실용 중국어 회화</t>
         </is>
       </c>
       <c r="D1432" t="inlineStr">
@@ -87793,15 +87817,19 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I1432" t="inlineStr"/>
+      <c r="I1432" t="inlineStr">
+        <is>
+          <t>안병삼</t>
+        </is>
+      </c>
       <c r="J1432" t="inlineStr">
         <is>
-          <t>수4~6</t>
+          <t>목2~4</t>
         </is>
       </c>
       <c r="K1432" t="inlineStr">
         <is>
-          <t>바울관403호강의실</t>
+          <t>미지정</t>
         </is>
       </c>
       <c r="L1432" t="inlineStr">
@@ -87815,17 +87843,17 @@
     <row r="1433">
       <c r="A1433" t="inlineStr">
         <is>
-          <t>522</t>
+          <t>499</t>
         </is>
       </c>
       <c r="B1433" t="inlineStr">
         <is>
-          <t>1006954</t>
+          <t>1002912</t>
         </is>
       </c>
       <c r="C1433" t="inlineStr">
         <is>
-          <t>일본인의 심리와 언어행동</t>
+          <t>실용일본어회화</t>
         </is>
       </c>
       <c r="D1433" t="inlineStr">
@@ -87849,19 +87877,15 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I1433" t="inlineStr">
-        <is>
-          <t>장성숙</t>
-        </is>
-      </c>
+      <c r="I1433" t="inlineStr"/>
       <c r="J1433" t="inlineStr">
         <is>
-          <t>수8~10</t>
+          <t>수4~6</t>
         </is>
       </c>
       <c r="K1433" t="inlineStr">
         <is>
-          <t>바울관402호강의실</t>
+          <t>바울관403호강의실</t>
         </is>
       </c>
       <c r="L1433" t="inlineStr">
@@ -87875,17 +87899,17 @@
     <row r="1434">
       <c r="A1434" t="inlineStr">
         <is>
-          <t>1654</t>
+          <t>522</t>
         </is>
       </c>
       <c r="B1434" t="inlineStr">
         <is>
-          <t>1007282</t>
+          <t>1006954</t>
         </is>
       </c>
       <c r="C1434" t="inlineStr">
         <is>
-          <t>항공관광실무영어Ⅱ</t>
+          <t>일본인의 심리와 언어행동</t>
         </is>
       </c>
       <c r="D1434" t="inlineStr">
@@ -87911,12 +87935,12 @@
       </c>
       <c r="I1434" t="inlineStr">
         <is>
-          <t>민세원</t>
+          <t>장성숙</t>
         </is>
       </c>
       <c r="J1434" t="inlineStr">
         <is>
-          <t>금2~4</t>
+          <t>수8~10</t>
         </is>
       </c>
       <c r="K1434" t="inlineStr">
@@ -87935,17 +87959,17 @@
     <row r="1435">
       <c r="A1435" t="inlineStr">
         <is>
-          <t>485</t>
+          <t>1654</t>
         </is>
       </c>
       <c r="B1435" t="inlineStr">
         <is>
-          <t>1005660</t>
+          <t>1007282</t>
         </is>
       </c>
       <c r="C1435" t="inlineStr">
         <is>
-          <t>현장어학실습 II</t>
+          <t>항공관광실무영어Ⅱ</t>
         </is>
       </c>
       <c r="D1435" t="inlineStr">
@@ -87971,12 +87995,12 @@
       </c>
       <c r="I1435" t="inlineStr">
         <is>
-          <t>안병삼</t>
+          <t>민세원</t>
         </is>
       </c>
       <c r="J1435" t="inlineStr">
         <is>
-          <t>목9~11</t>
+          <t>금2~4</t>
         </is>
       </c>
       <c r="K1435" t="inlineStr">
@@ -87995,17 +88019,17 @@
     <row r="1436">
       <c r="A1436" t="inlineStr">
         <is>
-          <t>504</t>
+          <t>485</t>
         </is>
       </c>
       <c r="B1436" t="inlineStr">
         <is>
-          <t>1004593</t>
+          <t>1005660</t>
         </is>
       </c>
       <c r="C1436" t="inlineStr">
         <is>
-          <t>졸업논문 및 중국어자격시험(신HSK6급)</t>
+          <t>현장어학실습 II</t>
         </is>
       </c>
       <c r="D1436" t="inlineStr">
@@ -88015,28 +88039,28 @@
       </c>
       <c r="E1436" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F1436" t="inlineStr">
         <is>
-          <t>전공필수</t>
+          <t>전공선택</t>
         </is>
       </c>
       <c r="G1436" t="inlineStr"/>
       <c r="H1436" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I1436" t="inlineStr">
         <is>
-          <t>김낙철</t>
+          <t>안병삼</t>
         </is>
       </c>
       <c r="J1436" t="inlineStr">
         <is>
-          <t>금8</t>
+          <t>목9~11</t>
         </is>
       </c>
       <c r="K1436" t="inlineStr">
@@ -88055,17 +88079,17 @@
     <row r="1437">
       <c r="A1437" t="inlineStr">
         <is>
-          <t>1158</t>
+          <t>504</t>
         </is>
       </c>
       <c r="B1437" t="inlineStr">
         <is>
-          <t>1004599</t>
+          <t>1004593</t>
         </is>
       </c>
       <c r="C1437" t="inlineStr">
         <is>
-          <t>졸업시험</t>
+          <t>졸업논문 및 중국어자격시험(신HSK6급)</t>
         </is>
       </c>
       <c r="D1437" t="inlineStr">
@@ -88091,17 +88115,17 @@
       </c>
       <c r="I1437" t="inlineStr">
         <is>
-          <t>유예진</t>
+          <t>김낙철</t>
         </is>
       </c>
       <c r="J1437" t="inlineStr">
         <is>
-          <t>금10</t>
+          <t>금8</t>
         </is>
       </c>
       <c r="K1437" t="inlineStr">
         <is>
-          <t>바울관403호강의실</t>
+          <t>바울관402호강의실</t>
         </is>
       </c>
       <c r="L1437" t="inlineStr">
@@ -88115,17 +88139,17 @@
     <row r="1438">
       <c r="A1438" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>1158</t>
         </is>
       </c>
       <c r="B1438" t="inlineStr">
         <is>
-          <t>1004601</t>
+          <t>1004599</t>
         </is>
       </c>
       <c r="C1438" t="inlineStr">
         <is>
-          <t>졸업연구</t>
+          <t>졸업시험</t>
         </is>
       </c>
       <c r="D1438" t="inlineStr">
@@ -88149,10 +88173,14 @@
           <t>0</t>
         </is>
       </c>
-      <c r="I1438" t="inlineStr"/>
+      <c r="I1438" t="inlineStr">
+        <is>
+          <t>유예진</t>
+        </is>
+      </c>
       <c r="J1438" t="inlineStr">
         <is>
-          <t>목11</t>
+          <t>금10</t>
         </is>
       </c>
       <c r="K1438" t="inlineStr">
@@ -88166,26 +88194,22 @@
         </is>
       </c>
       <c r="M1438" t="inlineStr"/>
-      <c r="N1438" t="inlineStr">
-        <is>
-          <t>(팀티칭)</t>
-        </is>
-      </c>
+      <c r="N1438" t="inlineStr"/>
     </row>
     <row r="1439">
       <c r="A1439" t="inlineStr">
         <is>
-          <t>1157</t>
+          <t>500</t>
         </is>
       </c>
       <c r="B1439" t="inlineStr">
         <is>
-          <t>1007131</t>
+          <t>1004601</t>
         </is>
       </c>
       <c r="C1439" t="inlineStr">
         <is>
-          <t>JLPT/JPT 및 졸업논문</t>
+          <t>졸업연구</t>
         </is>
       </c>
       <c r="D1439" t="inlineStr">
@@ -88200,28 +88224,24 @@
       </c>
       <c r="F1439" t="inlineStr">
         <is>
-          <t>전공선택</t>
+          <t>전공필수</t>
         </is>
       </c>
       <c r="G1439" t="inlineStr"/>
       <c r="H1439" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I1439" t="inlineStr">
-        <is>
-          <t>유예진</t>
-        </is>
-      </c>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I1439" t="inlineStr"/>
       <c r="J1439" t="inlineStr">
         <is>
-          <t>목9~11</t>
+          <t>목11</t>
         </is>
       </c>
       <c r="K1439" t="inlineStr">
         <is>
-          <t>바울관413호식음료실습실</t>
+          <t>바울관403호강의실</t>
         </is>
       </c>
       <c r="L1439" t="inlineStr">
@@ -88230,22 +88250,26 @@
         </is>
       </c>
       <c r="M1439" t="inlineStr"/>
-      <c r="N1439" t="inlineStr"/>
+      <c r="N1439" t="inlineStr">
+        <is>
+          <t>(팀티칭)</t>
+        </is>
+      </c>
     </row>
     <row r="1440">
       <c r="A1440" t="inlineStr">
         <is>
-          <t>1156</t>
+          <t>1157</t>
         </is>
       </c>
       <c r="B1440" t="inlineStr">
         <is>
-          <t>1007130</t>
+          <t>1007131</t>
         </is>
       </c>
       <c r="C1440" t="inlineStr">
         <is>
-          <t>신HSK 및 졸업논문</t>
+          <t>JLPT/JPT 및 졸업논문</t>
         </is>
       </c>
       <c r="D1440" t="inlineStr">
@@ -88271,17 +88295,17 @@
       </c>
       <c r="I1440" t="inlineStr">
         <is>
-          <t>박민수</t>
+          <t>유예진</t>
         </is>
       </c>
       <c r="J1440" t="inlineStr">
         <is>
-          <t>수9~11</t>
+          <t>목9~11</t>
         </is>
       </c>
       <c r="K1440" t="inlineStr">
         <is>
-          <t>바울관403호강의실</t>
+          <t>바울관413호식음료실습실</t>
         </is>
       </c>
       <c r="L1440" t="inlineStr">
@@ -88295,17 +88319,17 @@
     <row r="1441">
       <c r="A1441" t="inlineStr">
         <is>
-          <t>510</t>
+          <t>1156</t>
         </is>
       </c>
       <c r="B1441" t="inlineStr">
         <is>
-          <t>1002873</t>
+          <t>1007130</t>
         </is>
       </c>
       <c r="C1441" t="inlineStr">
         <is>
-          <t>실무중국어</t>
+          <t>신HSK 및 졸업논문</t>
         </is>
       </c>
       <c r="D1441" t="inlineStr">
@@ -88331,12 +88355,12 @@
       </c>
       <c r="I1441" t="inlineStr">
         <is>
-          <t>이성숙</t>
+          <t>박민수</t>
         </is>
       </c>
       <c r="J1441" t="inlineStr">
         <is>
-          <t>월2~4</t>
+          <t>수9~11</t>
         </is>
       </c>
       <c r="K1441" t="inlineStr">
@@ -88355,17 +88379,17 @@
     <row r="1442">
       <c r="A1442" t="inlineStr">
         <is>
-          <t>1653</t>
+          <t>510</t>
         </is>
       </c>
       <c r="B1442" t="inlineStr">
         <is>
-          <t>1004215</t>
+          <t>1002873</t>
         </is>
       </c>
       <c r="C1442" t="inlineStr">
         <is>
-          <t>일본어면접 및 취업준비</t>
+          <t>실무중국어</t>
         </is>
       </c>
       <c r="D1442" t="inlineStr">
@@ -88391,17 +88415,17 @@
       </c>
       <c r="I1442" t="inlineStr">
         <is>
-          <t>유예진</t>
+          <t>이성숙</t>
         </is>
       </c>
       <c r="J1442" t="inlineStr">
         <is>
-          <t>화2~4</t>
+          <t>월2~4</t>
         </is>
       </c>
       <c r="K1442" t="inlineStr">
         <is>
-          <t>바울관413호식음료실습실</t>
+          <t>바울관403호강의실</t>
         </is>
       </c>
       <c r="L1442" t="inlineStr">
@@ -88415,17 +88439,17 @@
     <row r="1443">
       <c r="A1443" t="inlineStr">
         <is>
-          <t>490</t>
+          <t>1653</t>
         </is>
       </c>
       <c r="B1443" t="inlineStr">
         <is>
-          <t>1004689</t>
+          <t>1004215</t>
         </is>
       </c>
       <c r="C1443" t="inlineStr">
         <is>
-          <t>중국어인터뷰</t>
+          <t>일본어면접 및 취업준비</t>
         </is>
       </c>
       <c r="D1443" t="inlineStr">
@@ -88451,17 +88475,17 @@
       </c>
       <c r="I1443" t="inlineStr">
         <is>
-          <t>안병삼</t>
+          <t>유예진</t>
         </is>
       </c>
       <c r="J1443" t="inlineStr">
         <is>
-          <t>수2~4</t>
+          <t>화2~4</t>
         </is>
       </c>
       <c r="K1443" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>바울관413호식음료실습실</t>
         </is>
       </c>
       <c r="L1443" t="inlineStr">
@@ -88475,17 +88499,17 @@
     <row r="1444">
       <c r="A1444" t="inlineStr">
         <is>
-          <t>502</t>
+          <t>490</t>
         </is>
       </c>
       <c r="B1444" t="inlineStr">
         <is>
-          <t>1007091</t>
+          <t>1004689</t>
         </is>
       </c>
       <c r="C1444" t="inlineStr">
         <is>
-          <t>항공관광서비스세미나(캡스톤디자인)</t>
+          <t>중국어인터뷰</t>
         </is>
       </c>
       <c r="D1444" t="inlineStr">
@@ -88511,17 +88535,17 @@
       </c>
       <c r="I1444" t="inlineStr">
         <is>
-          <t>김민주</t>
+          <t>안병삼</t>
         </is>
       </c>
       <c r="J1444" t="inlineStr">
         <is>
-          <t>수6~8</t>
+          <t>수2~4</t>
         </is>
       </c>
       <c r="K1444" t="inlineStr">
         <is>
-          <t>바울관403호강의실</t>
+          <t>미지정</t>
         </is>
       </c>
       <c r="L1444" t="inlineStr">
@@ -88535,17 +88559,17 @@
     <row r="1445">
       <c r="A1445" t="inlineStr">
         <is>
-          <t>1655</t>
+          <t>502</t>
         </is>
       </c>
       <c r="B1445" t="inlineStr">
         <is>
-          <t>1007293</t>
+          <t>1007091</t>
         </is>
       </c>
       <c r="C1445" t="inlineStr">
         <is>
-          <t>호텔업무론</t>
+          <t>항공관광서비스세미나(캡스톤디자인)</t>
         </is>
       </c>
       <c r="D1445" t="inlineStr">
@@ -88571,17 +88595,17 @@
       </c>
       <c r="I1445" t="inlineStr">
         <is>
-          <t>이효성</t>
+          <t>김민주</t>
         </is>
       </c>
       <c r="J1445" t="inlineStr">
         <is>
-          <t>화6~8</t>
+          <t>수6~8</t>
         </is>
       </c>
       <c r="K1445" t="inlineStr">
         <is>
-          <t>바울관402호강의실</t>
+          <t>바울관403호강의실</t>
         </is>
       </c>
       <c r="L1445" t="inlineStr">
@@ -88591,6 +88615,66 @@
       </c>
       <c r="M1445" t="inlineStr"/>
       <c r="N1445" t="inlineStr"/>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1655</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>1007293</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>호텔업무론</t>
+        </is>
+      </c>
+      <c r="D1446" t="inlineStr">
+        <is>
+          <t>항공관광외국어학부</t>
+        </is>
+      </c>
+      <c r="E1446" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F1446" t="inlineStr">
+        <is>
+          <t>전공선택</t>
+        </is>
+      </c>
+      <c r="G1446" t="inlineStr"/>
+      <c r="H1446" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I1446" t="inlineStr">
+        <is>
+          <t>이효성</t>
+        </is>
+      </c>
+      <c r="J1446" t="inlineStr">
+        <is>
+          <t>화6~8</t>
+        </is>
+      </c>
+      <c r="K1446" t="inlineStr">
+        <is>
+          <t>바울관402호강의실</t>
+        </is>
+      </c>
+      <c r="L1446" t="inlineStr">
+        <is>
+          <t>창의융합대학</t>
+        </is>
+      </c>
+      <c r="M1446" t="inlineStr"/>
+      <c r="N1446" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>